<commit_message>
Fix incorrect sort behavior and improve performance.
Sort didn't take into account types and the sorting was done thus incorrectly. It also used to use unstable sort. It now matches the sorting behavior of Excel (used in Dat - Sort and AutoFilter): numers, texts, logical, error and blank. Blank is always at the end, regardless of sorting order (asc/desc). Errors are not sorted.

The performance is improved by two-phase sorting: In first phase, only row indexes are sorted and we get a correct position of each row. That is done using BCL sorting algorithm O(N*log(N) * log(N) worst case because of stable sorting). After that, rows are swapped, so each row is sapped at most once O(N).
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
@@ -31,10 +31,10 @@
     <x:t>Names</x:t>
   </x:si>
   <x:si>
+    <x:t>Alex</x:t>
+  </x:si>
+  <x:si>
     <x:t>Jacques</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Alex</x:t>
   </x:si>
   <x:si>
     <x:t>Patrick</x:t>
@@ -456,7 +456,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:2">
+    <x:row r="2" spans="1:2" hidden="1">
       <x:c r="A2" s="0">
         <x:v>5</x:v>
       </x:c>
@@ -464,7 +464,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:2" hidden="1">
+    <x:row r="3" spans="1:2">
       <x:c r="A3" s="0">
         <x:v>5</x:v>
       </x:c>

</xml_diff>